<commit_message>
GetCareContact schema created. Updated service contract description and greening document for Vardkontakter
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/ehr/patientsummary/branches/TD_PATIENTSUMMARY_2/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vård- och omsorgskontak v6.xlsx
+++ b/ServiceInteractions/riv/ehr/patientsummary/branches/TD_PATIENTSUMMARY_2/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vård- och omsorgskontak v6.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14070" yWindow="-60" windowWidth="15195" windowHeight="12690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16580"/>
   </bookViews>
   <sheets>
     <sheet name="SendReferralAnswer CDA" sheetId="10" r:id="rId1"/>
     <sheet name="Blad1" sheetId="11" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="213">
   <si>
     <t>Meddelandestruktur</t>
   </si>
@@ -312,9 +317,6 @@
     <t>OID för Snomed CT</t>
   </si>
   <si>
-    <t>careDocumentationHeaderType</t>
-  </si>
-  <si>
     <t>Datattyp</t>
   </si>
   <si>
@@ -343,9 +345,6 @@
   </si>
   <si>
     <t>HSA-id för PDL-enhet</t>
-  </si>
-  <si>
-    <t>careContactType</t>
   </si>
   <si>
     <t>CareContactBodyType</t>
@@ -685,9 +684,6 @@
     <t>careContactStatus</t>
   </si>
   <si>
-    <t>careContactAddr</t>
-  </si>
-  <si>
     <t>careContactNamn</t>
   </si>
   <si>
@@ -698,6 +694,18 @@
   </si>
   <si>
     <t>careContactCode</t>
+  </si>
+  <si>
+    <t>CareContactHeaderType</t>
+  </si>
+  <si>
+    <t>CareContactType</t>
+  </si>
+  <si>
+    <t>careContactAddress</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -819,7 +827,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -827,13 +835,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color indexed="22"/>
@@ -858,7 +866,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1025,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1370,40 +1381,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Blad2">
+  <sheetPr codeName="Blad2" enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AY152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC83" sqref="AC83"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC80" sqref="AC80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
-    <col min="2" max="5" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="2.5" style="1" customWidth="1"/>
     <col min="6" max="8" width="3" style="1" customWidth="1"/>
-    <col min="9" max="12" width="3.42578125" style="1" customWidth="1"/>
-    <col min="13" max="17" width="3.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.5703125" style="1" customWidth="1"/>
+    <col min="9" max="12" width="3.5" style="1" customWidth="1"/>
+    <col min="13" max="17" width="3.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5" style="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="68.5703125" style="30" customWidth="1"/>
-    <col min="22" max="22" width="37.7109375" style="30" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="1"/>
-    <col min="24" max="24" width="10.28515625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.85546875" style="1"/>
-    <col min="29" max="29" width="24.7109375" style="1" customWidth="1"/>
-    <col min="30" max="30" width="19.5703125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="8.85546875" style="1"/>
+    <col min="20" max="20" width="20.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="68.5" style="30" customWidth="1"/>
+    <col min="22" max="22" width="37.6640625" style="30" customWidth="1"/>
+    <col min="23" max="23" width="8.83203125" style="1"/>
+    <col min="24" max="24" width="10.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="8.83203125" style="1"/>
+    <col min="29" max="29" width="24.6640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5" style="1" customWidth="1"/>
+    <col min="31" max="31" width="8.83203125" style="1"/>
     <col min="32" max="32" width="55" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="1"/>
+    <col min="33" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="2" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" s="2" customFormat="1" ht="3" customHeight="1">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1441,7 +1452,7 @@
       <c r="AI1" s="33"/>
       <c r="AN1" s="8"/>
     </row>
-    <row r="2" spans="1:40" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" ht="6.75" customHeight="1">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1483,7 +1494,7 @@
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
     </row>
-    <row r="3" spans="1:40" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" ht="27" customHeight="1">
       <c r="A3" s="65" t="s">
         <v>81</v>
       </c>
@@ -1524,7 +1535,7 @@
       <c r="AH3" s="66"/>
       <c r="AI3" s="66"/>
     </row>
-    <row r="4" spans="1:40" s="2" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" s="2" customFormat="1" ht="1.5" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -1561,7 +1572,7 @@
       <c r="AH4" s="32"/>
       <c r="AI4" s="32"/>
     </row>
-    <row r="5" spans="1:40" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" ht="30" customHeight="1">
       <c r="A5" s="62" t="s">
         <v>0</v>
       </c>
@@ -1583,14 +1594,14 @@
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
       <c r="S5" s="62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T5" s="14"/>
       <c r="U5" s="62" t="s">
         <v>34</v>
       </c>
       <c r="V5" s="62" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="W5" s="31"/>
       <c r="X5" s="31"/>
@@ -1599,20 +1610,20 @@
       <c r="AA5" s="31"/>
       <c r="AB5" s="64"/>
       <c r="AC5" s="64" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AD5" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE5" s="57" t="s">
         <v>96</v>
-      </c>
-      <c r="AE5" s="57" t="s">
-        <v>97</v>
       </c>
       <c r="AF5" s="46"/>
       <c r="AG5" s="31"/>
       <c r="AH5" s="31"/>
       <c r="AI5" s="31"/>
     </row>
-    <row r="6" spans="1:40" s="2" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" s="2" customFormat="1" ht="2.25" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -1649,7 +1660,7 @@
       <c r="AH6" s="35"/>
       <c r="AI6" s="35"/>
     </row>
-    <row r="7" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" ht="12.75" customHeight="1">
       <c r="A7" s="58" t="s">
         <v>80</v>
       </c>
@@ -1677,7 +1688,7 @@
       <c r="W7" s="36"/>
       <c r="AF7" s="30"/>
     </row>
-    <row r="8" spans="1:40" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="58" t="s">
         <v>44</v>
       </c>
@@ -1707,7 +1718,7 @@
       <c r="W8" s="17"/>
       <c r="AF8" s="29"/>
     </row>
-    <row r="9" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" s="2" customFormat="1">
       <c r="A9" s="58" t="s">
         <v>80</v>
       </c>
@@ -1733,11 +1744,11 @@
       <c r="U9" s="6"/>
       <c r="V9" s="49"/>
       <c r="W9" s="41" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="AF9" s="29"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40">
       <c r="A10" s="49" t="s">
         <v>6</v>
       </c>
@@ -1764,11 +1775,11 @@
       <c r="V10" s="42"/>
       <c r="W10" s="42"/>
       <c r="X10" s="17" t="s">
-        <v>95</v>
+        <v>209</v>
       </c>
       <c r="AF10" s="30"/>
     </row>
-    <row r="11" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" s="2" customFormat="1">
       <c r="A11" s="49"/>
       <c r="B11" s="49" t="s">
         <v>7</v>
@@ -1797,7 +1808,7 @@
       <c r="V11" s="29"/>
       <c r="AF11" s="29"/>
     </row>
-    <row r="12" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" s="2" customFormat="1">
       <c r="A12" s="49"/>
       <c r="B12" s="49"/>
       <c r="C12" s="49" t="s">
@@ -1831,7 +1842,7 @@
       <c r="V12" s="29"/>
       <c r="AF12" s="29"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40">
       <c r="A13" s="49"/>
       <c r="B13" s="49"/>
       <c r="C13" s="49" t="s">
@@ -1863,7 +1874,7 @@
       <c r="V13" s="49"/>
       <c r="AF13" s="30"/>
     </row>
-    <row r="14" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" s="2" customFormat="1">
       <c r="A14" s="49"/>
       <c r="B14" s="49" t="s">
         <v>8</v>
@@ -1889,28 +1900,28 @@
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="V14" s="50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="W14" s="3"/>
       <c r="Y14" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" s="2" customFormat="1">
       <c r="A15" s="49"/>
       <c r="B15" s="49"/>
       <c r="C15" s="49" t="s">
@@ -1944,7 +1955,7 @@
       <c r="Y15" s="3"/>
       <c r="AF15" s="29"/>
     </row>
-    <row r="16" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A16" s="49"/>
       <c r="B16" s="49"/>
       <c r="C16" s="49" t="s">
@@ -1979,7 +1990,7 @@
       <c r="Y16" s="3"/>
       <c r="AF16" s="29"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32">
       <c r="A17" s="49"/>
       <c r="B17" s="49" t="s">
         <v>9</v>
@@ -2009,7 +2020,7 @@
       <c r="Y17" s="3"/>
       <c r="AF17" s="30"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32">
       <c r="A18" s="49"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49" t="s">
@@ -2048,7 +2059,7 @@
       </c>
       <c r="AF18" s="61"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32">
       <c r="A19" s="49"/>
       <c r="B19" s="49"/>
       <c r="C19" s="49" t="s">
@@ -2082,7 +2093,7 @@
       <c r="Y19" s="3"/>
       <c r="AF19" s="30"/>
     </row>
-    <row r="20" spans="1:32" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" s="2" customFormat="1" ht="24">
       <c r="A20" s="49"/>
       <c r="B20" s="49" t="s">
         <v>24</v>
@@ -2108,18 +2119,18 @@
       </c>
       <c r="T20" s="15"/>
       <c r="U20" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V20" s="54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD20" s="3"/>
       <c r="AE20" s="3" t="s">
@@ -2129,7 +2140,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" s="2" customFormat="1">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
@@ -2157,14 +2168,14 @@
         <v>70</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="V21" s="54"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="AF21" s="29"/>
     </row>
-    <row r="22" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" s="2" customFormat="1">
       <c r="A22" s="15"/>
       <c r="B22" s="53" t="s">
         <v>32</v>
@@ -2193,7 +2204,7 @@
       <c r="V22" s="15"/>
       <c r="AF22" s="29"/>
     </row>
-    <row r="23" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" s="2" customFormat="1">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="53" t="s">
@@ -2227,7 +2238,7 @@
       <c r="V23" s="29"/>
       <c r="AF23" s="29"/>
     </row>
-    <row r="24" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" s="2" customFormat="1">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="53" t="s">
@@ -2259,7 +2270,7 @@
       <c r="V24" s="15"/>
       <c r="AF24" s="29"/>
     </row>
-    <row r="25" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" s="2" customFormat="1">
       <c r="A25" s="15"/>
       <c r="B25" s="53" t="s">
         <v>10</v>
@@ -2290,7 +2301,7 @@
       <c r="V25" s="29"/>
       <c r="AF25" s="29"/>
     </row>
-    <row r="26" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" s="2" customFormat="1">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="53" t="s">
@@ -2320,7 +2331,7 @@
       <c r="W26" s="3"/>
       <c r="AF26" s="29"/>
     </row>
-    <row r="27" spans="1:32" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" s="2" customFormat="1" ht="108">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="53"/>
@@ -2348,23 +2359,23 @@
       <c r="U27" s="8"/>
       <c r="V27" s="29"/>
       <c r="Y27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB27" s="3"/>
       <c r="AC27" s="40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AD27" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF27" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="AE27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF27" s="40" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:32" s="2" customFormat="1">
       <c r="A28" s="15"/>
       <c r="B28" s="53"/>
       <c r="C28" s="15"/>
@@ -2392,16 +2403,16 @@
         <v>70</v>
       </c>
       <c r="U28" s="25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V28" s="52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="X28" s="3"/>
       <c r="Y28" s="26"/>
       <c r="AF28" s="29"/>
     </row>
-    <row r="29" spans="1:32" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" s="2" customFormat="1" ht="24">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="53"/>
@@ -2434,7 +2445,7 @@
       <c r="V29" s="50"/>
       <c r="AF29" s="29"/>
     </row>
-    <row r="30" spans="1:32" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" s="2" customFormat="1" ht="24">
       <c r="A30" s="15"/>
       <c r="B30" s="15" t="s">
         <v>12</v>
@@ -2469,17 +2480,17 @@
       </c>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AF30" s="40" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" s="2" customFormat="1">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="53" t="s">
@@ -2514,7 +2525,7 @@
       <c r="AE31" s="3"/>
       <c r="AF31" s="50"/>
     </row>
-    <row r="32" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" s="2" customFormat="1">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2546,14 +2557,14 @@
       </c>
       <c r="V32" s="15"/>
       <c r="Z32" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD32" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE32" s="3" t="s">
         <v>1</v>
@@ -2562,7 +2573,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" s="2" customFormat="1">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
@@ -2596,7 +2607,7 @@
       <c r="AF33" s="50"/>
       <c r="AG33" s="26"/>
     </row>
-    <row r="34" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -2631,7 +2642,7 @@
       <c r="AE34" s="3"/>
       <c r="AF34" s="50"/>
     </row>
-    <row r="35" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" s="2" customFormat="1">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -2659,29 +2670,29 @@
         <v>70</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="V35" s="54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Z35" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AB35" s="3"/>
       <c r="AC35" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AD35" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE35" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AF35" s="40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2719,7 +2730,7 @@
       <c r="AE36" s="3"/>
       <c r="AF36" s="50"/>
     </row>
-    <row r="37" spans="1:33" s="2" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" s="2" customFormat="1" ht="58.5" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2752,24 +2763,24 @@
       <c r="V37" s="53"/>
       <c r="X37" s="4"/>
       <c r="Z37" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA37" s="4"/>
       <c r="AB37" s="5"/>
       <c r="AC37" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AD37" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AE37" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AF37" s="40" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2795,10 +2806,10 @@
       </c>
       <c r="T38" s="15"/>
       <c r="U38" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="V38" s="53" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AB38" s="3"/>
       <c r="AC38" s="3"/>
@@ -2806,7 +2817,7 @@
       <c r="AE38" s="3"/>
       <c r="AF38" s="50"/>
     </row>
-    <row r="39" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2843,7 +2854,7 @@
       <c r="AE39" s="3"/>
       <c r="AF39" s="50"/>
     </row>
-    <row r="40" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -2880,7 +2891,7 @@
       <c r="AE40" s="3"/>
       <c r="AF40" s="50"/>
     </row>
-    <row r="41" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -2913,7 +2924,7 @@
       <c r="AE41" s="3"/>
       <c r="AF41" s="50"/>
     </row>
-    <row r="42" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -2941,27 +2952,27 @@
         <v>70</v>
       </c>
       <c r="U42" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="V42" s="53" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB42" s="3"/>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AE42" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AF42" s="40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A43" s="15"/>
       <c r="B43" s="29"/>
       <c r="C43" s="15"/>
@@ -2994,7 +3005,7 @@
       <c r="AE43" s="3"/>
       <c r="AF43" s="50"/>
     </row>
-    <row r="44" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -3024,23 +3035,23 @@
       </c>
       <c r="V44" s="15"/>
       <c r="Z44" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AB44" s="3"/>
       <c r="AC44" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AD44" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AE44" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AF44" s="40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3071,7 +3082,7 @@
         <v>67</v>
       </c>
       <c r="V45" s="53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
@@ -3079,7 +3090,7 @@
       <c r="AE45" s="3"/>
       <c r="AF45" s="50"/>
     </row>
-    <row r="46" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3116,7 +3127,7 @@
       <c r="AE46" s="3"/>
       <c r="AF46" s="50"/>
     </row>
-    <row r="47" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3144,29 +3155,29 @@
         <v>70</v>
       </c>
       <c r="U47" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="V47" s="53" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
       <c r="AD47" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AE47" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AF47" s="40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AG47" s="3"/>
     </row>
-    <row r="48" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3194,7 +3205,7 @@
         <v>70</v>
       </c>
       <c r="U48" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="V48" s="53"/>
       <c r="Z48" s="3"/>
@@ -3204,7 +3215,7 @@
       <c r="AE48" s="3"/>
       <c r="AF48" s="50"/>
     </row>
-    <row r="49" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -3232,29 +3243,29 @@
         <v>70</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V49" s="53" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
       <c r="AD49" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AE49" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AF49" s="40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AG49" s="3"/>
     </row>
-    <row r="50" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -3289,7 +3300,7 @@
       <c r="AE50" s="3"/>
       <c r="AF50" s="50"/>
     </row>
-    <row r="51" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -3322,7 +3333,7 @@
       <c r="AE51" s="3"/>
       <c r="AF51" s="50"/>
     </row>
-    <row r="52" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -3357,7 +3368,7 @@
       <c r="AE52" s="3"/>
       <c r="AF52" s="50"/>
     </row>
-    <row r="53" spans="1:33" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -3385,29 +3396,29 @@
         <v>70</v>
       </c>
       <c r="U53" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V53" s="52" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Z53" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AB53" s="3"/>
       <c r="AC53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD53" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF53" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="AD53" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="AE53" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF53" s="40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
@@ -3444,7 +3455,7 @@
       <c r="AE54" s="3"/>
       <c r="AF54" s="50"/>
     </row>
-    <row r="55" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" s="2" customFormat="1">
       <c r="A55" s="15"/>
       <c r="B55" s="15" t="s">
         <v>16</v>
@@ -3482,7 +3493,7 @@
       <c r="AE55" s="3"/>
       <c r="AF55" s="40"/>
     </row>
-    <row r="56" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" s="2" customFormat="1">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15" t="s">
@@ -3518,7 +3529,7 @@
       <c r="AE56" s="3"/>
       <c r="AF56" s="40"/>
     </row>
-    <row r="57" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" s="2" customFormat="1">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
@@ -3554,7 +3565,7 @@
       <c r="AE57" s="3"/>
       <c r="AF57" s="40"/>
     </row>
-    <row r="58" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" s="2" customFormat="1">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
@@ -3592,7 +3603,7 @@
       <c r="AE58" s="3"/>
       <c r="AF58" s="40"/>
     </row>
-    <row r="59" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" s="2" customFormat="1">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
@@ -3620,10 +3631,10 @@
         <v>70</v>
       </c>
       <c r="U59" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="V59" s="53" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
@@ -3634,7 +3645,7 @@
       <c r="AE59" s="3"/>
       <c r="AF59" s="40"/>
     </row>
-    <row r="60" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" s="2" customFormat="1">
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
@@ -3675,10 +3686,10 @@
       <c r="AE60" s="3"/>
       <c r="AF60" s="40"/>
     </row>
-    <row r="61" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" s="2" customFormat="1">
       <c r="A61" s="15"/>
       <c r="B61" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
@@ -3701,28 +3712,28 @@
       </c>
       <c r="T61" s="15"/>
       <c r="U61" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="V61" s="40"/>
       <c r="W61" s="3"/>
       <c r="Y61" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Z61" s="3"/>
       <c r="AA61" s="3"/>
       <c r="AB61" s="3"/>
       <c r="AC61" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AD61" s="3"/>
       <c r="AE61" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AF61" s="40" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="62" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" s="2" customFormat="1">
       <c r="A62" s="15"/>
       <c r="B62" s="15"/>
       <c r="C62" s="53" t="s">
@@ -3758,7 +3769,7 @@
       <c r="AE62" s="3"/>
       <c r="AF62" s="40"/>
     </row>
-    <row r="63" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" s="2" customFormat="1" ht="24">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
@@ -3786,33 +3797,33 @@
         <v>70</v>
       </c>
       <c r="U63" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V63" s="54"/>
       <c r="Y63" s="3"/>
       <c r="Z63" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA63" s="3"/>
       <c r="AB63" s="3"/>
       <c r="AC63" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD63" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AE63" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AF63" s="55" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="64" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" s="2" customFormat="1">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="53" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
@@ -3845,12 +3856,12 @@
       <c r="AE64" s="3"/>
       <c r="AF64" s="40"/>
     </row>
-    <row r="65" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37" s="2" customFormat="1">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="53" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
@@ -3878,22 +3889,22 @@
       <c r="X65" s="3"/>
       <c r="Y65" s="3"/>
       <c r="Z65" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AA65" s="3"/>
       <c r="AB65" s="3"/>
       <c r="AC65" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AD65" s="3"/>
       <c r="AE65" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AF65" s="40" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="66" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37" s="2" customFormat="1">
       <c r="A66" s="15"/>
       <c r="B66" s="29"/>
       <c r="C66" s="15"/>
@@ -3918,7 +3929,7 @@
       <c r="V66" s="29"/>
       <c r="AF66" s="29"/>
     </row>
-    <row r="67" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:37" s="2" customFormat="1">
       <c r="A67" s="15"/>
       <c r="B67" s="29"/>
       <c r="C67" s="15"/>
@@ -3943,7 +3954,7 @@
       <c r="V67" s="53"/>
       <c r="AF67" s="29"/>
     </row>
-    <row r="68" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:37" s="2" customFormat="1">
       <c r="A68" s="15"/>
       <c r="B68" s="29"/>
       <c r="C68" s="15"/>
@@ -3968,7 +3979,7 @@
       <c r="V68" s="53"/>
       <c r="AF68" s="29"/>
     </row>
-    <row r="69" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:37" s="2" customFormat="1">
       <c r="A69" s="29"/>
       <c r="B69" s="60" t="s">
         <v>5</v>
@@ -3996,7 +4007,7 @@
       <c r="W69" s="3"/>
       <c r="AF69" s="29"/>
     </row>
-    <row r="70" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:37" s="2" customFormat="1">
       <c r="A70" s="29"/>
       <c r="B70" s="60" t="s">
         <v>19</v>
@@ -4022,11 +4033,11 @@
       <c r="U70" s="10"/>
       <c r="V70" s="15"/>
       <c r="X70" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AF70" s="29"/>
     </row>
-    <row r="71" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:37" s="2" customFormat="1">
       <c r="A71" s="29"/>
       <c r="B71" s="60" t="s">
         <v>5</v>
@@ -4067,7 +4078,7 @@
       <c r="AJ71" s="4"/>
       <c r="AK71" s="4"/>
     </row>
-    <row r="72" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:37" s="2" customFormat="1">
       <c r="A72" s="15"/>
       <c r="B72" s="15" t="s">
         <v>20</v>
@@ -4096,7 +4107,7 @@
       <c r="V72" s="15"/>
       <c r="AF72" s="29"/>
     </row>
-    <row r="73" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:37" s="4" customFormat="1">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15" t="s">
@@ -4125,7 +4136,7 @@
       <c r="V73" s="15"/>
       <c r="AF73" s="15"/>
     </row>
-    <row r="74" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:37" s="2" customFormat="1">
       <c r="A74" s="29"/>
       <c r="B74" s="60" t="s">
         <v>5</v>
@@ -4152,7 +4163,7 @@
       <c r="V74" s="15"/>
       <c r="AF74" s="29"/>
     </row>
-    <row r="75" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:37" s="2" customFormat="1">
       <c r="A75" s="29"/>
       <c r="B75" s="60" t="s">
         <v>48</v>
@@ -4179,7 +4190,7 @@
       <c r="V75" s="15"/>
       <c r="AF75" s="29"/>
     </row>
-    <row r="76" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:37" s="2" customFormat="1">
       <c r="A76" s="29"/>
       <c r="B76" s="60" t="s">
         <v>5</v>
@@ -4206,7 +4217,7 @@
       <c r="V76" s="15"/>
       <c r="AF76" s="29"/>
     </row>
-    <row r="77" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:37" s="2" customFormat="1">
       <c r="A77" s="15"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
@@ -4238,7 +4249,7 @@
       <c r="Y77" s="3"/>
       <c r="AF77" s="29"/>
     </row>
-    <row r="78" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:37" s="2" customFormat="1">
       <c r="A78" s="15"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -4267,7 +4278,7 @@
       <c r="V78" s="15"/>
       <c r="AF78" s="29"/>
     </row>
-    <row r="79" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:37" s="2" customFormat="1">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -4296,11 +4307,11 @@
         <v>62</v>
       </c>
       <c r="V79" s="54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AF79" s="29"/>
     </row>
-    <row r="80" spans="1:37" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:37" s="2" customFormat="1" ht="72">
       <c r="A80" s="15"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
@@ -4328,25 +4339,25 @@
         <v>70</v>
       </c>
       <c r="U80" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="V80" s="54"/>
       <c r="W80" s="3"/>
       <c r="Y80" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="AC80" s="3" t="s">
-        <v>179</v>
+        <v>208</v>
+      </c>
+      <c r="AC80" s="67" t="s">
+        <v>212</v>
       </c>
       <c r="AD80" s="3"/>
       <c r="AE80" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AF80" s="50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="81" spans="1:51" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:51" s="2" customFormat="1" ht="15">
       <c r="A81" s="15"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
@@ -4374,14 +4385,14 @@
         <v>92</v>
       </c>
       <c r="U81" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="V81" s="55"/>
       <c r="X81" s="3"/>
       <c r="Y81" s="26"/>
       <c r="AF81" s="29"/>
     </row>
-    <row r="82" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:51" s="2" customFormat="1">
       <c r="A82" s="15"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
@@ -4415,7 +4426,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:51" s="2" customFormat="1">
       <c r="A83" s="15"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
@@ -4441,14 +4452,14 @@
       </c>
       <c r="T83" s="15"/>
       <c r="U83" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="V83" s="54"/>
       <c r="X83" s="3"/>
       <c r="Y83" s="26"/>
       <c r="AF83" s="29"/>
     </row>
-    <row r="84" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:51" s="2" customFormat="1">
       <c r="A84" s="15"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
@@ -4477,7 +4488,7 @@
       <c r="Y84" s="26"/>
       <c r="AF84" s="29"/>
     </row>
-    <row r="85" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:51" s="2" customFormat="1">
       <c r="A85" s="15"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
@@ -4508,7 +4519,7 @@
       <c r="Y85" s="26"/>
       <c r="AF85" s="29"/>
     </row>
-    <row r="86" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:51" s="2" customFormat="1">
       <c r="A86" s="15"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
@@ -4539,7 +4550,7 @@
       <c r="Y86" s="26"/>
       <c r="AF86" s="29"/>
     </row>
-    <row r="87" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:51" s="2" customFormat="1">
       <c r="A87" s="15"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
@@ -4568,7 +4579,7 @@
       <c r="Y87" s="26"/>
       <c r="AF87" s="29"/>
     </row>
-    <row r="88" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:51" s="2" customFormat="1">
       <c r="A88" s="15"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
@@ -4591,17 +4602,17 @@
       <c r="R88" s="15"/>
       <c r="S88" s="53"/>
       <c r="T88" s="53" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U88" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="V88" s="54"/>
       <c r="X88" s="3"/>
       <c r="Y88" s="26"/>
       <c r="AF88" s="29"/>
     </row>
-    <row r="89" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:51" s="2" customFormat="1">
       <c r="A89" s="15"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
@@ -4634,7 +4645,7 @@
       <c r="Y89" s="26"/>
       <c r="AF89" s="29"/>
     </row>
-    <row r="90" spans="1:51" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:51" s="2" customFormat="1" ht="24">
       <c r="A90" s="15"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
@@ -4662,26 +4673,26 @@
         <v>70</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="V90" s="54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="X90" s="3"/>
       <c r="Y90" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AC90" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AE90" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AF90" s="63" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="91" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:51" s="2" customFormat="1">
       <c r="A91" s="15"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
@@ -4707,27 +4718,27 @@
       </c>
       <c r="T91" s="52"/>
       <c r="U91" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="V91" s="54" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="X91" s="3"/>
       <c r="Y91" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AC91" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD91" s="3"/>
       <c r="AE91" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AF91" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="92" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:51" s="2" customFormat="1">
       <c r="A92" s="15"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
@@ -4736,7 +4747,7 @@
       <c r="F92" s="53"/>
       <c r="G92" s="53"/>
       <c r="H92" s="53" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I92" s="15"/>
       <c r="J92" s="15"/>
@@ -4756,19 +4767,19 @@
       <c r="V92" s="54"/>
       <c r="X92" s="3"/>
       <c r="Y92" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AD92" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AE92" s="2" t="s">
         <v>4</v>
       </c>
       <c r="AF92" s="29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="93" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="93" spans="1:51" s="2" customFormat="1">
       <c r="A93" s="15"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
@@ -4778,7 +4789,7 @@
       <c r="G93" s="53"/>
       <c r="H93" s="59"/>
       <c r="I93" s="53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J93" s="15"/>
       <c r="K93" s="15"/>
@@ -4793,7 +4804,7 @@
         <v>1</v>
       </c>
       <c r="T93" s="53" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="U93" s="11"/>
       <c r="V93" s="54"/>
@@ -4801,7 +4812,7 @@
       <c r="Y93" s="3"/>
       <c r="AF93" s="29"/>
     </row>
-    <row r="94" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:51" s="2" customFormat="1">
       <c r="A94" s="15"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
@@ -4830,7 +4841,7 @@
       <c r="X94" s="3"/>
       <c r="AF94" s="29"/>
     </row>
-    <row r="95" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:51" s="2" customFormat="1">
       <c r="A95" s="15"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15"/>
@@ -4840,7 +4851,7 @@
       <c r="G95" s="53"/>
       <c r="H95" s="59"/>
       <c r="I95" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J95" s="29"/>
       <c r="K95" s="29"/>
@@ -4856,12 +4867,12 @@
       </c>
       <c r="T95" s="29"/>
       <c r="U95" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="X95" s="3"/>
       <c r="AF95" s="29"/>
     </row>
-    <row r="96" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:51" s="2" customFormat="1">
       <c r="A96" s="15"/>
       <c r="B96" s="15"/>
       <c r="C96" s="15"/>
@@ -4886,14 +4897,14 @@
         <v>1</v>
       </c>
       <c r="T96" s="52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U96" s="8"/>
       <c r="X96" s="3"/>
       <c r="Y96" s="3"/>
       <c r="AF96" s="29"/>
     </row>
-    <row r="97" spans="1:51" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:51" s="2" customFormat="1" ht="24">
       <c r="A97" s="15"/>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
@@ -4919,27 +4930,27 @@
       </c>
       <c r="T97" s="52"/>
       <c r="U97" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="V97" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="X97" s="3"/>
       <c r="Z97" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AC97" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AD97" s="3"/>
       <c r="AE97" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AF97" s="29" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="98" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:51" s="2" customFormat="1">
       <c r="A98" s="15"/>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
@@ -4967,7 +4978,7 @@
       <c r="Z98" s="3"/>
       <c r="AF98" s="29"/>
     </row>
-    <row r="99" spans="1:51" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:51" s="2" customFormat="1" ht="24">
       <c r="A99" s="15"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
@@ -4992,24 +5003,24 @@
       <c r="T99" s="52"/>
       <c r="U99" s="8"/>
       <c r="V99" s="54" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="X99" s="3"/>
       <c r="Z99" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AC99" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AD99" s="3"/>
       <c r="AE99" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AF99" s="29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="100" spans="1:51" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:51" s="2" customFormat="1" ht="24">
       <c r="A100" s="15"/>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
@@ -5034,24 +5045,24 @@
       <c r="T100" s="52"/>
       <c r="U100" s="8"/>
       <c r="V100" s="54" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X100" s="3"/>
-      <c r="Z100" s="3" t="s">
-        <v>207</v>
+      <c r="Z100" s="67" t="s">
+        <v>211</v>
       </c>
       <c r="AC100" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AD100" s="3"/>
       <c r="AE100" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AF100" s="29" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="101" spans="1:51" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="101" spans="1:51" s="2" customFormat="1" ht="24">
       <c r="A101" s="15"/>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -5075,10 +5086,10 @@
       <c r="S101" s="53"/>
       <c r="T101" s="52"/>
       <c r="U101" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="V101" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="X101" s="3"/>
       <c r="Z101" s="3"/>
@@ -5086,7 +5097,7 @@
       <c r="AD101" s="3"/>
       <c r="AF101" s="29"/>
     </row>
-    <row r="102" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:51" s="2" customFormat="1">
       <c r="A102" s="15"/>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>
@@ -5112,7 +5123,7 @@
       <c r="Y102" s="26"/>
       <c r="AF102" s="29"/>
     </row>
-    <row r="103" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:51" s="2" customFormat="1">
       <c r="A103" s="15"/>
       <c r="B103" s="29"/>
       <c r="C103" s="15"/>
@@ -5138,12 +5149,12 @@
       </c>
       <c r="T103" s="15"/>
       <c r="U103" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="V103" s="53"/>
       <c r="AF103" s="29"/>
     </row>
-    <row r="104" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:51" s="2" customFormat="1">
       <c r="A104" s="15"/>
       <c r="B104" s="15"/>
       <c r="C104" s="15"/>
@@ -5172,7 +5183,7 @@
       <c r="V104" s="15"/>
       <c r="AF104" s="29"/>
     </row>
-    <row r="105" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:51" s="2" customFormat="1">
       <c r="A105" s="15"/>
       <c r="B105" s="15"/>
       <c r="C105" s="15"/>
@@ -5201,7 +5212,7 @@
       <c r="V105" s="15"/>
       <c r="AF105" s="29"/>
     </row>
-    <row r="106" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:51" s="2" customFormat="1">
       <c r="A106" s="15"/>
       <c r="B106" s="15"/>
       <c r="C106" s="15"/>
@@ -5230,7 +5241,7 @@
       <c r="V106" s="55"/>
       <c r="AF106" s="29"/>
     </row>
-    <row r="107" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:51" s="2" customFormat="1">
       <c r="A107" s="15"/>
       <c r="B107" s="15"/>
       <c r="C107" s="15"/>
@@ -5239,7 +5250,7 @@
       <c r="F107" s="15"/>
       <c r="G107" s="15"/>
       <c r="H107" s="59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I107" s="15"/>
       <c r="J107" s="15"/>
@@ -5258,7 +5269,7 @@
       <c r="U107" s="12"/>
       <c r="AF107" s="29"/>
     </row>
-    <row r="108" spans="1:51" s="2" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:51" s="2" customFormat="1" ht="168">
       <c r="A108" s="15"/>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
@@ -5286,25 +5297,25 @@
         <v>70</v>
       </c>
       <c r="U108" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="V108" s="55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Y108" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AC108" s="2" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="AE108" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AF108" s="54" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="109" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="109" spans="1:51" s="2" customFormat="1">
       <c r="A109" s="15"/>
       <c r="B109" s="15"/>
       <c r="C109" s="15"/>
@@ -5329,7 +5340,7 @@
         <v>1</v>
       </c>
       <c r="T109" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U109" s="7" t="s">
         <v>93</v>
@@ -5340,7 +5351,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="110" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:51" s="2" customFormat="1">
       <c r="A110" s="15"/>
       <c r="B110" s="29"/>
       <c r="C110" s="15"/>
@@ -5368,7 +5379,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="111" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:51" s="2" customFormat="1">
       <c r="A111" s="15"/>
       <c r="B111" s="29"/>
       <c r="C111" s="29"/>
@@ -5396,7 +5407,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:51" s="2" customFormat="1">
       <c r="A112" s="15"/>
       <c r="B112" s="15" t="s">
         <v>5</v>
@@ -5426,7 +5437,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="113" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:51" s="2" customFormat="1">
       <c r="A113" s="15"/>
       <c r="B113" s="29"/>
       <c r="C113" s="29"/>
@@ -5454,7 +5465,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="114" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:51" s="2" customFormat="1">
       <c r="A114" s="15"/>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
@@ -5479,7 +5490,7 @@
       <c r="V114" s="55"/>
       <c r="AF114" s="29"/>
     </row>
-    <row r="115" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:51" s="2" customFormat="1">
       <c r="A115" s="15"/>
       <c r="B115" s="15"/>
       <c r="C115" s="15"/>
@@ -5504,7 +5515,7 @@
       <c r="V115" s="55"/>
       <c r="AF115" s="29"/>
     </row>
-    <row r="116" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:51" s="2" customFormat="1">
       <c r="A116" s="15"/>
       <c r="B116" s="15"/>
       <c r="C116" s="15"/>
@@ -5529,7 +5540,7 @@
       <c r="V116" s="15"/>
       <c r="AF116" s="29"/>
     </row>
-    <row r="117" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:51" s="2" customFormat="1">
       <c r="A117" s="15"/>
       <c r="B117" s="15"/>
       <c r="C117" s="15"/>
@@ -5554,7 +5565,7 @@
       <c r="V117" s="53"/>
       <c r="AF117" s="29"/>
     </row>
-    <row r="118" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:51" s="2" customFormat="1">
       <c r="A118" s="15"/>
       <c r="B118" s="15"/>
       <c r="C118" s="15"/>
@@ -5579,7 +5590,7 @@
       <c r="V118" s="53"/>
       <c r="AF118" s="29"/>
     </row>
-    <row r="119" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:51" s="2" customFormat="1">
       <c r="A119" s="15"/>
       <c r="B119" s="15"/>
       <c r="C119" s="15"/>
@@ -5604,7 +5615,7 @@
       <c r="V119" s="55"/>
       <c r="AF119" s="29"/>
     </row>
-    <row r="120" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:51" s="2" customFormat="1">
       <c r="A120" s="15"/>
       <c r="B120" s="15"/>
       <c r="C120" s="15"/>
@@ -5629,7 +5640,7 @@
       <c r="V120" s="15"/>
       <c r="AF120" s="29"/>
     </row>
-    <row r="121" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:51" s="2" customFormat="1">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -5654,7 +5665,7 @@
       <c r="V121" s="15"/>
       <c r="AF121" s="29"/>
     </row>
-    <row r="122" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:51" s="2" customFormat="1">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -5679,7 +5690,7 @@
       <c r="V122" s="15"/>
       <c r="AF122" s="29"/>
     </row>
-    <row r="123" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:51" s="2" customFormat="1">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -5704,7 +5715,7 @@
       <c r="V123" s="15"/>
       <c r="AF123" s="29"/>
     </row>
-    <row r="124" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:51" s="2" customFormat="1">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -5726,7 +5737,7 @@
       <c r="U124" s="29"/>
       <c r="V124" s="29"/>
     </row>
-    <row r="125" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:51" s="2" customFormat="1">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -5748,7 +5759,7 @@
       <c r="U125" s="15"/>
       <c r="V125" s="15"/>
     </row>
-    <row r="126" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:51" s="2" customFormat="1">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -5770,7 +5781,7 @@
       <c r="U126" s="15"/>
       <c r="V126" s="15"/>
     </row>
-    <row r="127" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:51" s="2" customFormat="1">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -5792,7 +5803,7 @@
       <c r="U127" s="15"/>
       <c r="V127" s="15"/>
     </row>
-    <row r="128" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:51" s="2" customFormat="1">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -5814,7 +5825,7 @@
       <c r="U128" s="15"/>
       <c r="V128" s="15"/>
     </row>
-    <row r="129" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:22" s="2" customFormat="1">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -5836,7 +5847,7 @@
       <c r="U129" s="53"/>
       <c r="V129" s="53"/>
     </row>
-    <row r="130" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:22" s="2" customFormat="1">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -5858,7 +5869,7 @@
       <c r="U130" s="55"/>
       <c r="V130" s="55"/>
     </row>
-    <row r="131" spans="1:22" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:22" s="2" customFormat="1" ht="26.25" customHeight="1">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -5880,7 +5891,7 @@
       <c r="U131" s="55"/>
       <c r="V131" s="55"/>
     </row>
-    <row r="132" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:22" s="2" customFormat="1">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -5901,7 +5912,7 @@
       <c r="U132" s="15"/>
       <c r="V132" s="15"/>
     </row>
-    <row r="133" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:22" s="2" customFormat="1">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -5921,7 +5932,7 @@
       <c r="U133" s="53"/>
       <c r="V133" s="53"/>
     </row>
-    <row r="134" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:22" s="2" customFormat="1">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -5943,7 +5954,7 @@
       <c r="U134" s="53"/>
       <c r="V134" s="53"/>
     </row>
-    <row r="135" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:22" s="2" customFormat="1">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -5966,73 +5977,73 @@
       <c r="U135" s="55"/>
       <c r="V135" s="55"/>
     </row>
-    <row r="136" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:22" s="2" customFormat="1">
       <c r="I136" s="3"/>
       <c r="U136" s="29"/>
       <c r="V136" s="29"/>
     </row>
-    <row r="137" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:22" s="2" customFormat="1">
       <c r="J137" s="3"/>
       <c r="U137" s="29"/>
       <c r="V137" s="29"/>
     </row>
-    <row r="138" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:22" s="2" customFormat="1">
       <c r="U138" s="29"/>
       <c r="V138" s="29"/>
     </row>
-    <row r="139" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:22" s="2" customFormat="1">
       <c r="U139" s="29"/>
       <c r="V139" s="29"/>
     </row>
-    <row r="140" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:22" s="2" customFormat="1">
       <c r="U140" s="29"/>
       <c r="V140" s="29"/>
     </row>
-    <row r="141" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:22" s="2" customFormat="1">
       <c r="U141" s="29"/>
       <c r="V141" s="29"/>
     </row>
-    <row r="142" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:22" s="2" customFormat="1">
       <c r="U142" s="29"/>
       <c r="V142" s="29"/>
     </row>
-    <row r="143" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:22" s="2" customFormat="1">
       <c r="U143" s="29"/>
       <c r="V143" s="29"/>
     </row>
-    <row r="144" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:22" s="2" customFormat="1">
       <c r="U144" s="29"/>
       <c r="V144" s="29"/>
     </row>
-    <row r="145" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="21:22" s="2" customFormat="1">
       <c r="U145" s="29"/>
       <c r="V145" s="29"/>
     </row>
-    <row r="146" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="21:22" s="2" customFormat="1">
       <c r="U146" s="29"/>
       <c r="V146" s="29"/>
     </row>
-    <row r="147" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="21:22" s="2" customFormat="1">
       <c r="U147" s="29"/>
       <c r="V147" s="29"/>
     </row>
-    <row r="148" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="21:22" s="2" customFormat="1">
       <c r="U148" s="29"/>
       <c r="V148" s="29"/>
     </row>
-    <row r="149" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="21:22" s="2" customFormat="1">
       <c r="U149" s="29"/>
       <c r="V149" s="29"/>
     </row>
-    <row r="150" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="21:22" s="2" customFormat="1">
       <c r="U150" s="29"/>
       <c r="V150" s="29"/>
     </row>
-    <row r="151" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="21:22" s="2" customFormat="1">
       <c r="U151" s="29"/>
       <c r="V151" s="29"/>
     </row>
-    <row r="152" spans="21:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="21:22" s="2" customFormat="1">
       <c r="U152" s="29"/>
       <c r="V152" s="29"/>
     </row>
@@ -6044,58 +6055,63 @@
     <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="8" scale="80" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="80" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Blad1"/>
+  <sheetPr codeName="Blad1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="47" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="48" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" s="48" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="48" t="s">
         <v>15</v>
       </c>
@@ -6113,5 +6129,10 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>